<commit_message>
Clean up of control_matrix integration
</commit_message>
<xml_diff>
--- a/integrations/controlmatrix/assets/data/controls_matrix.xlsx
+++ b/integrations/controlmatrix/assets/data/controls_matrix.xlsx
@@ -1,8 +1,19 @@
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E951F787-7BDA-4F62-A5EF-2251E7FF6B7C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02031BE9-CCF5-4DD2-B810-4994AFB56A3D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4cc75e8f-f493-4937-8b85-6d3b791ac2c2"/>
+    <ds:schemaRef ds:uri="1f05eadd-c3ed-4af1-86d9-17346ae05ad6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>